<commit_message>
fix: update scripts after 1st review
</commit_message>
<xml_diff>
--- a/Udacity_table_sizes.xlsx
+++ b/Udacity_table_sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larruda\source\udacity\WeatherReviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D23C62-87EE-4D5B-A184-264F3B6FCAD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18F8824-DA51-42D1-88B9-FC5E621102C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F3498627-A47E-4586-9986-B8DF5DE2C7C9}"/>
+    <workbookView xWindow="-27285" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{F3498627-A47E-4586-9986-B8DF5DE2C7C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>YELP_ACADEMIC_DATASET_BUSINESS.JSON</t>
   </si>
@@ -102,12 +102,6 @@
     <t>CHECKIN</t>
   </si>
   <si>
-    <t>TEMPERATURE</t>
-  </si>
-  <si>
-    <t>PRECIPITATION</t>
-  </si>
-  <si>
     <t>BUSINESS</t>
   </si>
   <si>
@@ -130,6 +124,9 @@
   </si>
   <si>
     <t>KB</t>
+  </si>
+  <si>
+    <t>WEATHER</t>
   </si>
 </sst>
 </file>
@@ -138,7 +135,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -188,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -272,13 +269,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -287,46 +323,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -344,7 +341,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -359,12 +356,49 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -375,52 +409,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -739,7 +785,7 @@
   <dimension ref="B1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,255 +814,251 @@
     <row r="2" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="20">
         <v>121466</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="20">
         <v>11852</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="8">
         <v>7933.5</v>
       </c>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="16">
+      <c r="C4" s="19"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="10">
         <v>3815</v>
       </c>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="16">
+      <c r="C5" s="19"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="10">
         <v>5537.5</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="15" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="10">
         <v>3835.5</v>
       </c>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="15" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="10">
         <v>740654.5</v>
       </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="12">
         <v>388938</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="13">
         <v>336201</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="10">
         <v>559421.5</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="12">
         <v>63316</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="13">
         <v>5007</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="16">
+      <c r="G9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="10">
         <v>5468.5</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="12">
         <v>6774100</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="13">
         <v>2660587</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="10">
         <v>2641133.5</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="12">
         <v>224910</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="13">
         <v>73842.5</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="10">
         <v>74052.5</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="12">
         <v>3598150</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="13">
         <v>2119419.5</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="10">
         <v>2116801.5</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="12">
         <v>517</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="13">
         <v>146</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="16">
-        <v>178.5</v>
+      <c r="G13" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="25">
+        <v>248</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="15">
         <v>800</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="17">
         <v>210.5</v>
       </c>
-      <c r="G14" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="24">
-        <v>225.5</v>
-      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="26"/>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -1039,37 +1081,40 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="24"/>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
@@ -1118,11 +1163,13 @@
       <c r="D47" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="H13:H14"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="F3:F7"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>